<commit_message>
Manual test case updated
</commit_message>
<xml_diff>
--- a/ManualTestCase_CreateWallet.xlsx
+++ b/ManualTestCase_CreateWallet.xlsx
@@ -5,23 +5,28 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Poorn\OneDrive\Desktop\TrustWallet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Poorn\OneDrive\Desktop\TrustWallet\sample-mobile-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECA5FBE4-97FF-4831-9652-F02162DBC739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0FE852-EC2B-467B-B746-ABC075C2C907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Browser Extension" sheetId="1" r:id="rId1"/>
-    <sheet name="Mobile" sheetId="2" r:id="rId2"/>
+    <sheet name="TC1" sheetId="3" r:id="rId2"/>
+    <sheet name="TC2" sheetId="4" r:id="rId3"/>
+    <sheet name="TC3" sheetId="5" r:id="rId4"/>
+    <sheet name="TC4" sheetId="6" r:id="rId5"/>
+    <sheet name="TC5" sheetId="7" r:id="rId6"/>
+    <sheet name="Mobile" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="281">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -494,12 +499,1988 @@
   <si>
     <t>TC_TW_032</t>
   </si>
+  <si>
+    <t>Test Case: Send Bitcoin - Show Error on Insufficient Balance</t>
+  </si>
+  <si>
+    <r>
+      <t>Test Case ID:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TC_SendBTC_001</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Module:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Send Cryptocurrency</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Priority:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> High</t>
+    </r>
+  </si>
+  <si>
+    <t>Preconditions:</t>
+  </si>
+  <si>
+    <t>User has successfully created and logged into their Interest Wallet.</t>
+  </si>
+  <si>
+    <t>Wallet balance for BTC is 0.</t>
+  </si>
+  <si>
+    <t>A valid BTC wallet address is available or saved.</t>
+  </si>
+  <si>
+    <t>Test Steps:</t>
+  </si>
+  <si>
+    <t>Step No</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Launch the Interest Wallet app.</t>
+  </si>
+  <si>
+    <t>App opens and lands on Home screen.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tap on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Send"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> button from the Home screen.</t>
+    </r>
+  </si>
+  <si>
+    <t>Navigates to the "Select Asset to Send" screen.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Select </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bitcoin (BTC)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from the asset list.</t>
+    </r>
+  </si>
+  <si>
+    <t>Navigates to the "Send BTC" screen.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tap on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Add Address"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> if no saved addresses are available.</t>
+    </r>
+  </si>
+  <si>
+    <t>Navigates to the "Add New Address" screen.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>wallet name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g., "MyWallet") and select BTC as the asset.</t>
+    </r>
+  </si>
+  <si>
+    <t>BTC selected and wallet name entered.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>valid BTC address</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g., 17... format).</t>
+    </r>
+  </si>
+  <si>
+    <t>BTC address input is accepted.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tap on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Done"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> after entering the address.</t>
+    </r>
+  </si>
+  <si>
+    <t>Address is saved successfully and user is taken back to Send BTC screen.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>$500</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Amount</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> field.</t>
+    </r>
+  </si>
+  <si>
+    <t>Amount is entered.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tap </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Next"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Continue"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to proceed with the transaction.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Error message shown: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Not enough balance"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Expected Result:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When the user tries to send $500 worth of BTC with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 BTC balance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, the app should display a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>clear error message</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> such as:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"Not enough balance"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Insufficient funds"</t>
+    </r>
+  </si>
+  <si>
+    <t>The transaction should not proceed.</t>
+  </si>
+  <si>
+    <t>Postconditions:</t>
+  </si>
+  <si>
+    <t>No transaction is performed.</t>
+  </si>
+  <si>
+    <t>Wallet balance remains unchanged.</t>
+  </si>
+  <si>
+    <t>Test Case: View History When No Transactions Exist</t>
+  </si>
+  <si>
+    <r>
+      <t>Test Case ID:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TC_History_001</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Module:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Transaction History</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Priority:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Medium</t>
+    </r>
+  </si>
+  <si>
+    <t>User is logged into the Interest Wallet.</t>
+  </si>
+  <si>
+    <t>No crypto or NFT transactions (send, receive, buy) have been made.</t>
+  </si>
+  <si>
+    <t>App opens and lands on the Home screen.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tap on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>History icon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> at the top-left corner.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Navigates to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Transaction History</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page.</t>
+    </r>
+  </si>
+  <si>
+    <t>Observe the screen contents.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Message displayed: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"No transaction available"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Can't find any transaction?"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tap on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Check Explorer"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> link.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Navigates to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Explorer page</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Review the data shown on the Explorer page.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Displays wallet summary info: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>total balance, received, buy amount, etc.</t>
+    </r>
+  </si>
+  <si>
+    <t>Expected Results:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If no transactions have been made, the history screen should clearly indicate that </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>no transactions are available</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Check Explorer"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> link should redirect to a summary page that shows:</t>
+    </r>
+  </si>
+  <si>
+    <t>Total Balance</t>
+  </si>
+  <si>
+    <t>Amount Bought</t>
+  </si>
+  <si>
+    <t>Amount Received</t>
+  </si>
+  <si>
+    <t>Any other relevant wallet info (e.g., number of assets)</t>
+  </si>
+  <si>
+    <t>No data is modified; only read/view operations are performed.</t>
+  </si>
+  <si>
+    <t>Test Case: View and Filter Trending Coins</t>
+  </si>
+  <si>
+    <r>
+      <t>Test Case ID:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TC_Trending_001</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Module:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Trending</t>
+    </r>
+  </si>
+  <si>
+    <t>Internet connection is available.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tap on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Trending"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> menu option.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Navigates to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Trending</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> screen.</t>
+    </r>
+  </si>
+  <si>
+    <t>Observe the dropdown at the top-left corner of the screen.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dropdown with two options: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"1 Hour"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"24 Hours"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is visible.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Select </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"24 Hours"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from the dropdown.</t>
+    </r>
+  </si>
+  <si>
+    <t>Trending data for the past 24 hours is displayed (e.g., for Bitcoin, ETH, etc).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Select </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"1 Hour"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from the dropdown.</t>
+    </r>
+  </si>
+  <si>
+    <t>Trending data for the last 1 hour is updated and shown.</t>
+  </si>
+  <si>
+    <t>View the trending coins list and analyze one coin (e.g., Bitcoin).</t>
+  </si>
+  <si>
+    <t>The price change (e.g., +2.3%) over the selected timeframe is shown.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Check if there's a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>map or chart form</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of trend data.</t>
+    </r>
+  </si>
+  <si>
+    <t>Visual representation (chart or graph) of the trend is visible.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Explore filter for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>networks</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g., all networks vs specific networks).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User can toggle to view data for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>specific networks</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>all</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tap on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Download</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Export</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> icon (if available).</t>
+    </r>
+  </si>
+  <si>
+    <t>Data is downloadable as per app capability.</t>
+  </si>
+  <si>
+    <r>
+      <t>Trending screen should correctly update based on the selected timeframe (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 hour / 24 hours</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Each coin's trend should show </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>percentage change</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>visual chart</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>network info</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Dropdown filter should work seamlessly.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The ability to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>filter by network</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> should update the trend list accordingly.</t>
+    </r>
+  </si>
+  <si>
+    <t>Data should be relevant for crypto buying decisions.</t>
+  </si>
+  <si>
+    <t>No changes made to user data or wallet; only view operations performed.</t>
+  </si>
+  <si>
+    <t>Test Case: Swap Tokens - Show Error on Insufficient Balance</t>
+  </si>
+  <si>
+    <r>
+      <t>Test Case ID:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TC_Swap_001</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Module:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Swap</t>
+    </r>
+  </si>
+  <si>
+    <t>Wallet balance for selected source asset (e.g., BNB) is 0 or less than the swap amount.</t>
+  </si>
+  <si>
+    <t>Launch the Interest Wallet app and land on the Home screen.</t>
+  </si>
+  <si>
+    <t>Home screen is displayed.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tap on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Swap"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> button.</t>
+    </r>
+  </si>
+  <si>
+    <t>Navigates to the Swap screen.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"From"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> field, select </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BNB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (or another source asset).</t>
+    </r>
+  </si>
+  <si>
+    <t>Asset selection is updated.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"To"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> field, select another token (e.g., BTC, USDT).</t>
+    </r>
+  </si>
+  <si>
+    <t>Destination asset is updated.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>random amount</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> greater than current balance (e.g., 5 BNB).</t>
+    </r>
+  </si>
+  <si>
+    <t>Amount field is populated.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Observe the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>comparison/conversion field</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>App calculates and shows equivalent amount in destination token (if possible).</t>
+  </si>
+  <si>
+    <t>Try to proceed with the swap.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Error message is shown: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Insufficient balance"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in red.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The swap screen should show a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>real-time conversion</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> between the selected assets based on current exchange rates.</t>
+    </r>
+  </si>
+  <si>
+    <t>If the amount entered exceeds available balance:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">An error </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Balance exceeded"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Insufficient balance"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> should appear in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>red</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Swap action should be </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>disabled or blocked</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> until the issue is resolved.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Optionally, the app can show a suggestion like </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Buy more BNB to proceed with swap."</t>
+    </r>
+  </si>
+  <si>
+    <t>No swap is executed.</t>
+  </si>
+  <si>
+    <t>Test Case: Search and View Asset Details</t>
+  </si>
+  <si>
+    <r>
+      <t>Test Case ID:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TC_Search_001</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Module:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Search</t>
+    </r>
+  </si>
+  <si>
+    <t>Internet connection is active.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tap on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Search icon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (usually on top-right).</t>
+    </r>
+  </si>
+  <si>
+    <t>Search bar or screen with a list of all available assets is displayed.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Browse or type an asset name (e.g., </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bitcoin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) in the search bar.</t>
+    </r>
+  </si>
+  <si>
+    <t>Matching assets are filtered and shown in real-time.</t>
+  </si>
+  <si>
+    <t>Tap on a specific asset from the list.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Navigates to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Asset Detail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> screen.</t>
+    </r>
+  </si>
+  <si>
+    <t>Observe the asset detail page.</t>
+  </si>
+  <si>
+    <t>Page shows:</t>
+  </si>
+  <si>
+    <t>Current Price</t>
+  </si>
+  <si>
+    <t>Trend chart</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Available actions: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Buy, Sell, Swap, Gift</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. |</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">| 6 | Tap on any action (e.g., </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Buy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Swap</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) from the asset detail screen. | Navigates to respective action screen with the selected asset pre-filled. |</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User should be able to search and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>find assets quickly</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Selecting an asset shows </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>complete information</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, including:</t>
+    </r>
+  </si>
+  <si>
+    <t>Live price</t>
+  </si>
+  <si>
+    <t>Trend/graph</t>
+  </si>
+  <si>
+    <t>Description or symbol details</t>
+  </si>
+  <si>
+    <r>
+      <t>Action buttons (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Buy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sell</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Swap</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gift</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Tapping on any action redirects to the correct flow with that asset selected.</t>
+  </si>
+  <si>
+    <t>No changes made to wallet unless a user proceeds with a transaction from an action button.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -517,6 +2498,22 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -557,12 +2554,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -879,7 +2899,7 @@
     <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="65.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1145,7 +3165,7 @@
       <c r="D18" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" t="s">
         <v>137</v>
       </c>
     </row>
@@ -1197,10 +3217,1227 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D6FA43-C91A-48C6-92D7-359E26CF7B27}">
+  <dimension ref="A1:C43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A18" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="32.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="32.77734375" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="54" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+    </row>
+    <row r="8" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+    </row>
+    <row r="12" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>2</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>3</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>4</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>5</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>6</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>7</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>8</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>9</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+    </row>
+    <row r="32" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F42CBA1C-93EF-41C6-B1C4-652A8D880A21}">
+  <dimension ref="A1:C44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="32.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="32.77734375" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>1</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>3</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>4</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>5</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="8"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="9"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="8"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
+    </row>
+    <row r="44" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC73BD7-4AE2-4AB9-A0DA-D7935F06A242}">
+  <dimension ref="A1:C44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="32.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="32.77734375" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>1</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>3</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>4</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>5</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>6</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>7</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>8</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>9</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+    </row>
+    <row r="32" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="9"/>
+    </row>
+    <row r="34" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+    </row>
+    <row r="36" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="8"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
+    </row>
+    <row r="44" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EAD2DC4-0885-407E-A34B-E4A00A0978E8}">
+  <dimension ref="A1:C56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="32.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="32.77734375" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="54" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>1</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>3</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>4</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>5</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>6</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>7</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="9"/>
+    </row>
+    <row r="34" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+    </row>
+    <row r="36" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="8"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="49" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="50" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="51" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="52" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="53" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="55" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="56" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16275011-9AE7-4AE9-8F44-65DF9642F828}">
+  <dimension ref="A1:C56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="32.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="32.77734375" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>1</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>3</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>4</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>5</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="29" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="73.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="9"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+    </row>
+    <row r="36" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="8"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3D9804-21DC-4598-A89E-D2E5DEEC78B1}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -1401,36 +4638,36 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>146</v>
       </c>
       <c r="B12" t="s">
         <v>144</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
         <v>138</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" t="s">
         <v>139</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>147</v>
       </c>
       <c r="B13" t="s">
         <v>145</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" t="s">
         <v>141</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" t="s">
         <v>142</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" t="s">
         <v>143</v>
       </c>
     </row>

</xml_diff>